<commit_message>
save dulu done ya
</commit_message>
<xml_diff>
--- a/LEFO Market Research/LEFO MR 2024/Quarto dan Epoxy/hasil tabulasi new.xlsx
+++ b/LEFO Market Research/LEFO MR 2024/Quarto dan Epoxy/hasil tabulasi new.xlsx
@@ -737,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>250</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5">
@@ -782,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>50</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="10">
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="n">
-        <v>50</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="11">
@@ -827,7 +827,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16">
@@ -838,7 +838,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>250</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17">
@@ -860,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>50</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="19">
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>50</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="20">
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="13" t="n">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24">
@@ -911,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="13" t="n">
-        <v>250</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25">
@@ -933,7 +933,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="13" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
@@ -944,7 +944,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="13" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
@@ -955,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="13" t="n">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29">
@@ -966,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
@@ -977,7 +977,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="13" t="n">
-        <v>343</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31">
@@ -1026,13 +1026,13 @@
         <v>10</v>
       </c>
       <c r="C36" s="23" t="n">
-        <v>2.8</v>
+        <v>5.55555555555556</v>
       </c>
       <c r="D36" s="17" t="n">
-        <v>6</v>
+        <v>2.25563909774436</v>
       </c>
       <c r="E36" s="25" t="n">
-        <v>4.4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="37">
@@ -1043,13 +1043,13 @@
         <v>11</v>
       </c>
       <c r="C37" s="23" t="n">
-        <v>8.8</v>
+        <v>6.83760683760684</v>
       </c>
       <c r="D37" s="17" t="n">
-        <v>7.6</v>
+        <v>7.14285714285714</v>
       </c>
       <c r="E37" s="25" t="n">
-        <v>8.2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1060,13 +1060,13 @@
         <v>12</v>
       </c>
       <c r="C38" s="23" t="n">
-        <v>14.8</v>
+        <v>17.9487179487179</v>
       </c>
       <c r="D38" s="17" t="n">
-        <v>12.4</v>
+        <v>15.7894736842105</v>
       </c>
       <c r="E38" s="25" t="n">
-        <v>13.6</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="39">
@@ -1077,13 +1077,13 @@
         <v>13</v>
       </c>
       <c r="C39" s="23" t="n">
-        <v>5.6</v>
+        <v>7.69230769230769</v>
       </c>
       <c r="D39" s="17" t="n">
-        <v>4.8</v>
+        <v>7.14285714285714</v>
       </c>
       <c r="E39" s="25" t="n">
-        <v>5.2</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="40">
@@ -1094,13 +1094,13 @@
         <v>14</v>
       </c>
       <c r="C40" s="23" t="n">
-        <v>68</v>
+        <v>61.965811965812</v>
       </c>
       <c r="D40" s="17" t="n">
-        <v>69.2</v>
+        <v>67.6691729323308</v>
       </c>
       <c r="E40" s="25" t="n">
-        <v>68.6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41">
@@ -1111,10 +1111,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="24" t="n">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="D41" s="19" t="n">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="E41" s="26" t="n">
         <v>500</v>
@@ -1155,13 +1155,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="29" t="n">
-        <v>50</v>
+        <v>48.546511627907</v>
       </c>
       <c r="D46" s="27" t="n">
-        <v>50</v>
+        <v>42.9487179487179</v>
       </c>
       <c r="E46" s="31" t="n">
-        <v>50</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="47">
@@ -1172,13 +1172,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="29" t="n">
-        <v>50</v>
+        <v>51.453488372093</v>
       </c>
       <c r="D47" s="27" t="n">
-        <v>50</v>
+        <v>57.0512820512821</v>
       </c>
       <c r="E47" s="31" t="n">
-        <v>50</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="48">
@@ -1189,10 +1189,10 @@
         <v>6</v>
       </c>
       <c r="C48" s="30" t="n">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D48" s="28" t="n">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E48" s="32" t="n">
         <v>500</v>
@@ -1214,7 +1214,7 @@
         <v>21</v>
       </c>
       <c r="B52" s="33" t="n">
-        <v>91.1111111111111</v>
+        <v>91.1646586345382</v>
       </c>
     </row>
     <row r="53">
@@ -1222,7 +1222,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="33" t="n">
-        <v>71.1111111111111</v>
+        <v>69.4779116465863</v>
       </c>
     </row>
     <row r="54">
@@ -1230,7 +1230,7 @@
         <v>23</v>
       </c>
       <c r="B54" s="33" t="n">
-        <v>53.5353535353535</v>
+        <v>49.1967871485944</v>
       </c>
     </row>
     <row r="55">
@@ -1238,7 +1238,7 @@
         <v>24</v>
       </c>
       <c r="B55" s="33" t="n">
-        <v>27.8787878787879</v>
+        <v>28.1124497991968</v>
       </c>
     </row>
     <row r="56">
@@ -1246,7 +1246,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="33" t="n">
-        <v>1.01010101010101</v>
+        <v>1.40562248995984</v>
       </c>
     </row>
     <row r="57">
@@ -1254,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="34" t="n">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="59">
@@ -1287,13 +1287,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="37" t="n">
-        <v>91.1290322580645</v>
+        <v>92.7038626609442</v>
       </c>
       <c r="C62" s="35" t="n">
-        <v>91.0931174089069</v>
+        <v>89.811320754717</v>
       </c>
       <c r="D62" s="39" t="n">
-        <v>91.1111111111111</v>
+        <v>91.1646586345382</v>
       </c>
     </row>
     <row r="63">
@@ -1301,13 +1301,13 @@
         <v>22</v>
       </c>
       <c r="B63" s="37" t="n">
-        <v>70.5645161290323</v>
+        <v>66.9527896995708</v>
       </c>
       <c r="C63" s="35" t="n">
-        <v>71.6599190283401</v>
+        <v>71.6981132075472</v>
       </c>
       <c r="D63" s="39" t="n">
-        <v>71.1111111111111</v>
+        <v>69.4779116465863</v>
       </c>
     </row>
     <row r="64">
@@ -1315,13 +1315,13 @@
         <v>23</v>
       </c>
       <c r="B64" s="37" t="n">
-        <v>50.8064516129032</v>
+        <v>47.2103004291845</v>
       </c>
       <c r="C64" s="35" t="n">
-        <v>56.2753036437247</v>
+        <v>50.9433962264151</v>
       </c>
       <c r="D64" s="39" t="n">
-        <v>53.5353535353535</v>
+        <v>49.1967871485944</v>
       </c>
     </row>
     <row r="65">
@@ -1329,13 +1329,13 @@
         <v>24</v>
       </c>
       <c r="B65" s="37" t="n">
-        <v>28.2258064516129</v>
+        <v>31.7596566523605</v>
       </c>
       <c r="C65" s="35" t="n">
-        <v>27.5303643724696</v>
+        <v>24.9056603773585</v>
       </c>
       <c r="D65" s="39" t="n">
-        <v>27.8787878787879</v>
+        <v>28.1124497991968</v>
       </c>
     </row>
     <row r="66">
@@ -1343,13 +1343,13 @@
         <v>25</v>
       </c>
       <c r="B66" s="37" t="n">
-        <v>1.20967741935484</v>
+        <v>0.858369098712446</v>
       </c>
       <c r="C66" s="35" t="n">
-        <v>0.809716599190283</v>
+        <v>1.88679245283019</v>
       </c>
       <c r="D66" s="39" t="n">
-        <v>1.01010101010101</v>
+        <v>1.40562248995984</v>
       </c>
     </row>
     <row r="67">
@@ -1357,13 +1357,13 @@
         <v>6</v>
       </c>
       <c r="B67" s="38" t="n">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="C67" s="36" t="n">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="D67" s="40" t="n">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="69">
@@ -1412,13 +1412,13 @@
         <v>14</v>
       </c>
       <c r="C73" s="46" t="n">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D73" s="42" t="n">
-        <v>69.2</v>
+        <v>67.7</v>
       </c>
       <c r="E73" s="48" t="n">
-        <v>68.6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74">
@@ -1429,13 +1429,13 @@
         <v>12</v>
       </c>
       <c r="C74" s="46" t="n">
-        <v>14.8</v>
+        <v>17.9</v>
       </c>
       <c r="D74" s="42" t="n">
-        <v>12.4</v>
+        <v>15.8</v>
       </c>
       <c r="E74" s="48" t="n">
-        <v>13.6</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="75">
@@ -1443,16 +1443,16 @@
         <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C75" s="46" t="n">
-        <v>8.8</v>
+        <v>7.7</v>
       </c>
       <c r="D75" s="42" t="n">
-        <v>7.6</v>
+        <v>7.1</v>
       </c>
       <c r="E75" s="48" t="n">
-        <v>8.2</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="76">
@@ -1460,16 +1460,16 @@
         <v>4</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C76" s="46" t="n">
-        <v>5.6</v>
+        <v>6.8</v>
       </c>
       <c r="D76" s="42" t="n">
-        <v>4.8</v>
+        <v>7.1</v>
       </c>
       <c r="E76" s="48" t="n">
-        <v>5.2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -1480,13 +1480,13 @@
         <v>10</v>
       </c>
       <c r="C77" s="46" t="n">
-        <v>2.8</v>
+        <v>5.6</v>
       </c>
       <c r="D77" s="42" t="n">
-        <v>6</v>
+        <v>2.3</v>
       </c>
       <c r="E77" s="48" t="n">
-        <v>4.4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="78">
@@ -1497,10 +1497,10 @@
         <v>6</v>
       </c>
       <c r="C78" s="47" t="n">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="D78" s="43" t="n">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="E78" s="49" t="n">
         <v>500</v>

</xml_diff>

<commit_message>
save politik untuk sharing ke sma 1
</commit_message>
<xml_diff>
--- a/LEFO Market Research/LEFO MR 2024/Quarto dan Epoxy/hasil tabulasi new.xlsx
+++ b/LEFO Market Research/LEFO MR 2024/Quarto dan Epoxy/hasil tabulasi new.xlsx
@@ -737,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5">
@@ -782,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>50.8</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="10">
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="n">
-        <v>49.2</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="11">
@@ -827,7 +827,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16">
@@ -838,7 +838,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17">
@@ -860,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>50.8</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="19">
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>49.2</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="20">
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="13" t="n">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24">
@@ -911,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="13" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25">
@@ -933,7 +933,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="13" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
@@ -944,7 +944,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="13" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28">
@@ -955,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="13" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29">
@@ -966,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30">
@@ -977,7 +977,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="13" t="n">
-        <v>355</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31">
@@ -1026,13 +1026,13 @@
         <v>10</v>
       </c>
       <c r="C36" s="23" t="n">
-        <v>3.1496062992126</v>
+        <v>2.89256198347107</v>
       </c>
       <c r="D36" s="17" t="n">
-        <v>2.03252032520325</v>
+        <v>4.26356589147287</v>
       </c>
       <c r="E36" s="25" t="n">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="37">
@@ -1043,13 +1043,13 @@
         <v>11</v>
       </c>
       <c r="C37" s="23" t="n">
-        <v>5.11811023622047</v>
+        <v>9.91735537190083</v>
       </c>
       <c r="D37" s="17" t="n">
-        <v>6.09756097560976</v>
+        <v>7.36434108527132</v>
       </c>
       <c r="E37" s="25" t="n">
-        <v>5.6</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="38">
@@ -1060,13 +1060,13 @@
         <v>12</v>
       </c>
       <c r="C38" s="23" t="n">
-        <v>13.3858267716535</v>
+        <v>11.1570247933884</v>
       </c>
       <c r="D38" s="17" t="n">
-        <v>12.1951219512195</v>
+        <v>15.1162790697674</v>
       </c>
       <c r="E38" s="25" t="n">
-        <v>12.8</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="39">
@@ -1077,13 +1077,13 @@
         <v>13</v>
       </c>
       <c r="C39" s="23" t="n">
-        <v>9.44881889763779</v>
+        <v>9.91735537190083</v>
       </c>
       <c r="D39" s="17" t="n">
-        <v>6.50406504065041</v>
+        <v>5.81395348837209</v>
       </c>
       <c r="E39" s="25" t="n">
-        <v>8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="40">
@@ -1094,13 +1094,13 @@
         <v>14</v>
       </c>
       <c r="C40" s="23" t="n">
-        <v>68.8976377952756</v>
+        <v>66.1157024793389</v>
       </c>
       <c r="D40" s="17" t="n">
-        <v>73.1707317073171</v>
+        <v>67.4418604651163</v>
       </c>
       <c r="E40" s="25" t="n">
-        <v>71</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="41">
@@ -1111,10 +1111,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="24" t="n">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D41" s="19" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="E41" s="26" t="n">
         <v>500</v>
@@ -1155,13 +1155,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="29" t="n">
-        <v>49.7237569060773</v>
+        <v>47.9166666666667</v>
       </c>
       <c r="D46" s="27" t="n">
-        <v>53.6231884057971</v>
+        <v>49.390243902439</v>
       </c>
       <c r="E46" s="31" t="n">
-        <v>50.8</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="47">
@@ -1172,13 +1172,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="29" t="n">
-        <v>50.2762430939227</v>
+        <v>52.0833333333333</v>
       </c>
       <c r="D47" s="27" t="n">
-        <v>46.3768115942029</v>
+        <v>50.609756097561</v>
       </c>
       <c r="E47" s="31" t="n">
-        <v>49.2</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="48">
@@ -1189,10 +1189,10 @@
         <v>6</v>
       </c>
       <c r="C48" s="30" t="n">
-        <v>362</v>
+        <v>336</v>
       </c>
       <c r="D48" s="28" t="n">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E48" s="32" t="n">
         <v>500</v>
@@ -1214,7 +1214,7 @@
         <v>21</v>
       </c>
       <c r="B52" s="33" t="n">
-        <v>94.5454545454545</v>
+        <v>90.3420523138833</v>
       </c>
     </row>
     <row r="53">
@@ -1222,7 +1222,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="33" t="n">
-        <v>71.3131313131313</v>
+        <v>72.0321931589537</v>
       </c>
     </row>
     <row r="54">
@@ -1230,7 +1230,7 @@
         <v>23</v>
       </c>
       <c r="B54" s="33" t="n">
-        <v>48.0808080808081</v>
+        <v>49.8993963782696</v>
       </c>
     </row>
     <row r="55">
@@ -1238,7 +1238,7 @@
         <v>24</v>
       </c>
       <c r="B55" s="33" t="n">
-        <v>32.3232323232323</v>
+        <v>29.1750503018109</v>
       </c>
     </row>
     <row r="56">
@@ -1246,7 +1246,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="33" t="n">
-        <v>0.606060606060606</v>
+        <v>1.40845070422535</v>
       </c>
     </row>
     <row r="57">
@@ -1254,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="34" t="n">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="59">
@@ -1287,13 +1287,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="37" t="n">
-        <v>92.8286852589641</v>
+        <v>90.495867768595</v>
       </c>
       <c r="C62" s="35" t="n">
-        <v>96.3114754098361</v>
+        <v>90.1960784313726</v>
       </c>
       <c r="D62" s="39" t="n">
-        <v>94.5454545454545</v>
+        <v>90.3420523138833</v>
       </c>
     </row>
     <row r="63">
@@ -1301,13 +1301,13 @@
         <v>22</v>
       </c>
       <c r="B63" s="37" t="n">
-        <v>73.3067729083665</v>
+        <v>71.0743801652893</v>
       </c>
       <c r="C63" s="35" t="n">
-        <v>69.2622950819672</v>
+        <v>72.9411764705882</v>
       </c>
       <c r="D63" s="39" t="n">
-        <v>71.3131313131313</v>
+        <v>72.0321931589537</v>
       </c>
     </row>
     <row r="64">
@@ -1315,13 +1315,13 @@
         <v>23</v>
       </c>
       <c r="B64" s="37" t="n">
-        <v>48.605577689243</v>
+        <v>51.2396694214876</v>
       </c>
       <c r="C64" s="35" t="n">
-        <v>47.5409836065574</v>
+        <v>48.6274509803922</v>
       </c>
       <c r="D64" s="39" t="n">
-        <v>48.0808080808081</v>
+        <v>49.8993963782696</v>
       </c>
     </row>
     <row r="65">
@@ -1329,13 +1329,13 @@
         <v>24</v>
       </c>
       <c r="B65" s="37" t="n">
-        <v>29.8804780876494</v>
+        <v>29.7520661157025</v>
       </c>
       <c r="C65" s="35" t="n">
-        <v>34.8360655737705</v>
+        <v>28.6274509803922</v>
       </c>
       <c r="D65" s="39" t="n">
-        <v>32.3232323232323</v>
+        <v>29.1750503018109</v>
       </c>
     </row>
     <row r="66">
@@ -1343,11 +1343,13 @@
         <v>25</v>
       </c>
       <c r="B66" s="37" t="n">
-        <v>1.19521912350598</v>
-      </c>
-      <c r="C66" s="35"/>
+        <v>2.06611570247934</v>
+      </c>
+      <c r="C66" s="35" t="n">
+        <v>0.784313725490196</v>
+      </c>
       <c r="D66" s="39" t="n">
-        <v>0.606060606060606</v>
+        <v>1.40845070422535</v>
       </c>
     </row>
     <row r="67">
@@ -1355,13 +1357,13 @@
         <v>6</v>
       </c>
       <c r="B67" s="38" t="n">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C67" s="36" t="n">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="D67" s="40" t="n">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="69">
@@ -1410,13 +1412,13 @@
         <v>14</v>
       </c>
       <c r="C73" s="46" t="n">
-        <v>68.9</v>
+        <v>66.1</v>
       </c>
       <c r="D73" s="42" t="n">
-        <v>73.2</v>
+        <v>67.4</v>
       </c>
       <c r="E73" s="48" t="n">
-        <v>71</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="74">
@@ -1427,13 +1429,13 @@
         <v>12</v>
       </c>
       <c r="C74" s="46" t="n">
-        <v>13.4</v>
+        <v>11.2</v>
       </c>
       <c r="D74" s="42" t="n">
-        <v>12.2</v>
+        <v>15.1</v>
       </c>
       <c r="E74" s="48" t="n">
-        <v>12.8</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="75">
@@ -1441,16 +1443,16 @@
         <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C75" s="46" t="n">
-        <v>9.4</v>
+        <v>9.9</v>
       </c>
       <c r="D75" s="42" t="n">
-        <v>6.5</v>
+        <v>7.4</v>
       </c>
       <c r="E75" s="48" t="n">
-        <v>8</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="76">
@@ -1458,16 +1460,16 @@
         <v>4</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76" s="46" t="n">
-        <v>5.1</v>
+        <v>9.9</v>
       </c>
       <c r="D76" s="42" t="n">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="E76" s="48" t="n">
-        <v>5.6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="77">
@@ -1478,13 +1480,13 @@
         <v>10</v>
       </c>
       <c r="C77" s="46" t="n">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="D77" s="42" t="n">
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="E77" s="48" t="n">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="78">
@@ -1495,10 +1497,10 @@
         <v>6</v>
       </c>
       <c r="C78" s="47" t="n">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D78" s="43" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="E78" s="49" t="n">
         <v>500</v>

</xml_diff>